<commit_message>
test PR with a new version of concept
In the new excel file a concept elter_dl:04 is deleted and a new concept elter_dl:06 is created
</commit_message>
<xml_diff>
--- a/dataLevel.xlsx
+++ b/dataLevel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrooggioni/Sites/GitHub/elter-vocabularies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F646B16-D31F-864A-86B9-A2A5A1EDE4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673D08EA-433E-1A40-A70F-70FA38A44077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41780" yWindow="-3900" windowWidth="28800" windowHeight="16640" tabRatio="652" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-41780" yWindow="-3900" windowWidth="28800" windowHeight="16640" tabRatio="652" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="146">
   <si>
     <t>Vocabulary IRI*</t>
   </si>
@@ -1662,9 +1662,6 @@
     <t>elter_dl:03</t>
   </si>
   <si>
-    <t>elter_dl:04</t>
-  </si>
-  <si>
     <t>observation data</t>
   </si>
   <si>
@@ -1731,19 +1728,10 @@
     <t>https://ror.org/02wxw4x45</t>
   </si>
   <si>
-    <t>model product</t>
-  </si>
-  <si>
-    <t>an example of the new concept</t>
-  </si>
-  <si>
-    <t>level 4</t>
-  </si>
-  <si>
-    <t>eLTER_dl:06</t>
-  </si>
-  <si>
-    <t>elter_dl:01, elter_dl:02, elter_dl:03, elter_dl:04, elter_dl:06</t>
+    <t>elter_dl:06</t>
+  </si>
+  <si>
+    <t>elter_dl:01, elter_dl:02, elter_dl:03, elter_dl:06</t>
   </si>
 </sst>
 </file>
@@ -2587,8 +2575,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}" name="concepts" displayName="concepts" ref="A2:I20" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A2:I20" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}" name="concepts" displayName="concepts" ref="A2:I19" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A2:I19" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{9FE8BFF8-A78B-448D-A131-9A0D98C9F3D7}" name="Concept IRI*" dataDxfId="33"/>
     <tableColumn id="2" xr3:uid="{86239A34-9941-49E0-9977-1A07DF28C21F}" name="Preferred Label*" dataDxfId="32"/>
@@ -2993,7 +2981,7 @@
         <v>37</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5872,7 +5860,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>69</v>
@@ -5942,7 +5930,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>46</v>
@@ -5956,7 +5944,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>46</v>
@@ -7022,10 +7010,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7080,23 +7068,23 @@
         <v>120</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I3" s="23"/>
     </row>
@@ -7105,23 +7093,23 @@
         <v>121</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I4" s="24"/>
     </row>
@@ -7130,74 +7118,60 @@
         <v>122</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I5" s="23"/>
     </row>
-    <row r="6" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>48</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>147</v>
-      </c>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="23"/>
-      <c r="H7" s="23" t="s">
-        <v>139</v>
-      </c>
+      <c r="H7" s="23"/>
       <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -7331,17 +7305,6 @@
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
       <c r="I19" s="23"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7897,8 +7860,8 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7934,19 +7897,19 @@
     </row>
     <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="D3" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="23" t="s">
         <v>137</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -8111,7 +8074,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
         <v>119</v>

</xml_diff>